<commit_message>
AM session update to murhocomparison, new att-calc figures
</commit_message>
<xml_diff>
--- a/gamma/data-table-shiedling.xlsx
+++ b/gamma/data-table-shiedling.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\GarrettandJordan-gamma\king-stomps-phy451\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\GarrettandJordan-gamma\king-stomps-phy451\gamma\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,8 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="Pb" sheetId="1" r:id="rId1"/>
-    <sheet name="energy-v-murho" sheetId="5" r:id="rId2"/>
-    <sheet name="Error analysis" sheetId="4" r:id="rId3"/>
+    <sheet name="Al" sheetId="6" r:id="rId2"/>
+    <sheet name="energy-v-murho" sheetId="5" r:id="rId3"/>
+    <sheet name="Error analysis" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Thickness (mm)</t>
   </si>
@@ -50,6 +51,12 @@
   </si>
   <si>
     <t>error (cm^2/g)</t>
+  </si>
+  <si>
+    <t>Pb Data</t>
+  </si>
+  <si>
+    <t>Al Data</t>
   </si>
 </sst>
 </file>
@@ -371,7 +378,7 @@
   <dimension ref="A1:C89"/>
   <sheetViews>
     <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79:C85"/>
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,10 +1291,537 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="A2:C8"/>
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>663.1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>19083</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>663.1</v>
+      </c>
+      <c r="B3">
+        <v>6.47</v>
+      </c>
+      <c r="C3">
+        <v>16840</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>663.1</v>
+      </c>
+      <c r="B4">
+        <v>12.89</v>
+      </c>
+      <c r="C4">
+        <v>14785</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>663.1</v>
+      </c>
+      <c r="B5">
+        <v>19.64</v>
+      </c>
+      <c r="C5">
+        <v>12729</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>663.1</v>
+      </c>
+      <c r="B6">
+        <v>26.2</v>
+      </c>
+      <c r="C6">
+        <v>11098</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>663.1</v>
+      </c>
+      <c r="B7">
+        <v>38.909999999999997</v>
+      </c>
+      <c r="C7">
+        <v>8591</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1173.2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>2919</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1173.2</v>
+      </c>
+      <c r="B9">
+        <v>6.47</v>
+      </c>
+      <c r="C9">
+        <v>2635</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1173.2</v>
+      </c>
+      <c r="B10">
+        <v>12.89</v>
+      </c>
+      <c r="C10">
+        <v>2208</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1173.2</v>
+      </c>
+      <c r="B11">
+        <v>19.64</v>
+      </c>
+      <c r="C11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1173.2</v>
+      </c>
+      <c r="B12">
+        <v>26.2</v>
+      </c>
+      <c r="C12">
+        <v>1818</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1173.2</v>
+      </c>
+      <c r="B13">
+        <v>38.909999999999997</v>
+      </c>
+      <c r="C13">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1332.5</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1332.5</v>
+      </c>
+      <c r="B15">
+        <v>6.47</v>
+      </c>
+      <c r="C15">
+        <v>2194</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1332.5</v>
+      </c>
+      <c r="B16">
+        <v>12.89</v>
+      </c>
+      <c r="C16">
+        <v>1934</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1332.5</v>
+      </c>
+      <c r="B17">
+        <v>19.64</v>
+      </c>
+      <c r="C17">
+        <v>1654</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1332.5</v>
+      </c>
+      <c r="B18">
+        <v>26.2</v>
+      </c>
+      <c r="C18">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1332.5</v>
+      </c>
+      <c r="B19">
+        <v>38.909999999999997</v>
+      </c>
+      <c r="C19">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>80.998000000000005</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>3505</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>80.998000000000005</v>
+      </c>
+      <c r="B21">
+        <v>6.47</v>
+      </c>
+      <c r="C21">
+        <v>2603</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>80.998000000000005</v>
+      </c>
+      <c r="B22">
+        <v>12.89</v>
+      </c>
+      <c r="C22">
+        <v>1748</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>80.998000000000005</v>
+      </c>
+      <c r="B23">
+        <v>19.64</v>
+      </c>
+      <c r="C23">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>80.998000000000005</v>
+      </c>
+      <c r="B24">
+        <v>26.2</v>
+      </c>
+      <c r="C24">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>80.998000000000005</v>
+      </c>
+      <c r="B25">
+        <v>38.909999999999997</v>
+      </c>
+      <c r="C25">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>276.39699999999999</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>276.39699999999999</v>
+      </c>
+      <c r="B27">
+        <v>6.47</v>
+      </c>
+      <c r="C27">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>276.39699999999999</v>
+      </c>
+      <c r="B28">
+        <v>12.89</v>
+      </c>
+      <c r="C28">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>276.39699999999999</v>
+      </c>
+      <c r="B29">
+        <v>19.64</v>
+      </c>
+      <c r="C29">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>276.39699999999999</v>
+      </c>
+      <c r="B30">
+        <v>26.2</v>
+      </c>
+      <c r="C30">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>276.39699999999999</v>
+      </c>
+      <c r="B31">
+        <v>38.909999999999997</v>
+      </c>
+      <c r="C31">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>302.851</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>302.851</v>
+      </c>
+      <c r="B33">
+        <v>6.47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>302.851</v>
+      </c>
+      <c r="B34">
+        <v>12.89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>302.851</v>
+      </c>
+      <c r="B35">
+        <v>19.64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>302.851</v>
+      </c>
+      <c r="B36">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>302.851</v>
+      </c>
+      <c r="B37">
+        <v>38.909999999999997</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>356.005</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>356.005</v>
+      </c>
+      <c r="B39">
+        <v>6.47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>356.005</v>
+      </c>
+      <c r="B40">
+        <v>12.89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>356.005</v>
+      </c>
+      <c r="B41">
+        <v>19.64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>356.005</v>
+      </c>
+      <c r="B42">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>356.005</v>
+      </c>
+      <c r="B43">
+        <v>38.909999999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>383.851</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>383.851</v>
+      </c>
+      <c r="B45">
+        <v>6.47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>383.851</v>
+      </c>
+      <c r="B46">
+        <v>12.89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>383.851</v>
+      </c>
+      <c r="B47">
+        <v>19.64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>383.851</v>
+      </c>
+      <c r="B48">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>383.851</v>
+      </c>
+      <c r="B49">
+        <v>38.909999999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="1"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="1"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B79" s="1"/>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B89" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1296,7 +1830,7 @@
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1307,7 +1841,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>276.39699999999999</v>
       </c>
@@ -1315,11 +1849,11 @@
         <v>0.40810000000000002</v>
       </c>
       <c r="C2">
-        <f>(0.0197+0.068)*B2</f>
-        <v>3.5790370000000002E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <f>(0.068)*B2</f>
+        <v>2.7750800000000003E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>302.851</v>
       </c>
@@ -1327,11 +1861,14 @@
         <v>0.34210000000000002</v>
       </c>
       <c r="C3">
-        <f>B3*(0.0197+0.033)</f>
-        <v>1.802867E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <f>B3*(0.033)</f>
+        <v>1.12893E-2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>356.005</v>
       </c>
@@ -1339,11 +1876,11 @@
         <v>0.25090000000000001</v>
       </c>
       <c r="C4">
-        <f>B4*(0.0197+0.017)</f>
-        <v>9.208029999999999E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <f>B4*(0.017)</f>
+        <v>4.2653000000000005E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>383.851</v>
       </c>
@@ -1351,11 +1888,11 @@
         <v>0.2041</v>
       </c>
       <c r="C5">
-        <f>B5*(0.0197+0.043)</f>
-        <v>1.2797069999999999E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <f>B5*(0.043)</f>
+        <v>8.776299999999999E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>661.7</v>
       </c>
@@ -1363,11 +1900,11 @@
         <v>9.7199999999999995E-2</v>
       </c>
       <c r="C6">
-        <f>B6*(0.0197+0.0108)</f>
-        <v>2.9646E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <f>B6*(0.0108)</f>
+        <v>1.0497600000000001E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1173.2</v>
       </c>
@@ -1375,11 +1912,11 @@
         <v>6.9400000000000003E-2</v>
       </c>
       <c r="C7">
-        <f>B7*(0.0197+0.063)</f>
-        <v>5.7393799999999997E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <f>B7*(0.063)</f>
+        <v>4.3722000000000006E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1332.5</v>
       </c>
@@ -1387,8 +1924,72 @@
         <v>5.11E-2</v>
       </c>
       <c r="C8">
-        <f>B8*(0.0197+0.04)</f>
-        <v>3.0506700000000001E-3</v>
+        <f>B8*(0.04)</f>
+        <v>2.0439999999999998E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>80.998000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>276.39699999999999</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>302.851</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>356.005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>383.851</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>661.7</v>
+      </c>
+      <c r="B17">
+        <v>5.45E-2</v>
+      </c>
+      <c r="C17">
+        <f>B17*0.0844</f>
+        <v>4.5998000000000002E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1173.2</v>
+      </c>
+      <c r="B18">
+        <v>7.6399999999999996E-2</v>
+      </c>
+      <c r="C18">
+        <f>B18*0.2617</f>
+        <v>1.9993879999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1332.5</v>
+      </c>
+      <c r="B19">
+        <v>7.8899999999999998E-2</v>
+      </c>
+      <c r="C19">
+        <f>B19*0.2155</f>
+        <v>1.7002949999999999E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1396,7 +1997,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>

</xml_diff>

<commit_message>
Pm session-- updated 133Ba plots and the spreadsheet with 12 min data for 133Ba
</commit_message>
<xml_diff>
--- a/gamma/data-table-shiedling.xlsx
+++ b/gamma/data-table-shiedling.xlsx
@@ -1293,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1522,7 +1522,8 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <v>3505</v>
+        <f>3505+7115</f>
+        <v>10620</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1533,7 +1534,8 @@
         <v>6.47</v>
       </c>
       <c r="C21">
-        <v>2603</v>
+        <f>4795+2603</f>
+        <v>7398</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1544,7 +1546,8 @@
         <v>12.89</v>
       </c>
       <c r="C22">
-        <v>1748</v>
+        <f>3366+1748</f>
+        <v>5114</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1555,7 +1558,8 @@
         <v>19.64</v>
       </c>
       <c r="C23">
-        <v>1376</v>
+        <f>2258+1376</f>
+        <v>3634</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1566,7 +1570,8 @@
         <v>26.2</v>
       </c>
       <c r="C24">
-        <v>999</v>
+        <f>1666+999</f>
+        <v>2665</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1577,7 +1582,8 @@
         <v>38.909999999999997</v>
       </c>
       <c r="C25">
-        <v>556</v>
+        <f>910+556</f>
+        <v>1466</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1588,7 +1594,8 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <v>705</v>
+        <f>1470+705</f>
+        <v>2175</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1599,7 +1606,8 @@
         <v>6.47</v>
       </c>
       <c r="C27">
-        <v>624</v>
+        <f>1155+624</f>
+        <v>1779</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1610,7 +1618,8 @@
         <v>12.89</v>
       </c>
       <c r="C28">
-        <v>480</v>
+        <f>994+480</f>
+        <v>1474</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1621,7 +1630,8 @@
         <v>19.64</v>
       </c>
       <c r="C29">
-        <v>459</v>
+        <f>779+459</f>
+        <v>1238</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1632,7 +1642,8 @@
         <v>26.2</v>
       </c>
       <c r="C30">
-        <v>386</v>
+        <f>627+386</f>
+        <v>1013</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1643,7 +1654,8 @@
         <v>38.909999999999997</v>
       </c>
       <c r="C31">
-        <v>252</v>
+        <f>408+252</f>
+        <v>660</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1653,147 +1665,219 @@
       <c r="B32" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <f>3184+1693</f>
+        <v>4877</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>302.851</v>
       </c>
       <c r="B33">
         <v>6.47</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <f>2365+1384</f>
+        <v>3749</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>302.851</v>
       </c>
       <c r="B34">
         <v>12.89</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <f>1951+1179</f>
+        <v>3130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>302.851</v>
       </c>
       <c r="B35">
         <v>19.64</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <f>1481+1069</f>
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>302.851</v>
       </c>
       <c r="B36">
         <v>26.2</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <f>1369+787</f>
+        <v>2156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>302.851</v>
       </c>
       <c r="B37">
         <v>38.909999999999997</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <f>984+538</f>
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>356.005</v>
       </c>
       <c r="B38" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <f>7919+4649</f>
+        <v>12568</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>356.005</v>
       </c>
       <c r="B39">
         <v>6.47</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <f>6273+3813</f>
+        <v>10086</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>356.005</v>
       </c>
       <c r="B40">
         <v>12.89</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <f>5204+3188</f>
+        <v>8392</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>356.005</v>
       </c>
       <c r="B41">
         <v>19.64</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <f>4116+2665</f>
+        <v>6781</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>356.005</v>
       </c>
       <c r="B42">
         <v>26.2</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <f>3800+2185</f>
+        <v>5985</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>356.005</v>
       </c>
       <c r="B43">
         <v>38.909999999999997</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <f>2653+1600</f>
+        <v>4253</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>383.851</v>
       </c>
       <c r="B44" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <f>1070+552</f>
+        <v>1622</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>383.851</v>
       </c>
       <c r="B45">
         <v>6.47</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <f>860+542</f>
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>383.851</v>
       </c>
       <c r="B46">
         <v>12.89</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <f>763+420</f>
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>383.851</v>
       </c>
       <c r="B47">
         <v>19.64</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <f>587+364</f>
+        <v>951</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>383.851</v>
       </c>
       <c r="B48">
         <v>26.2</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <f>497+270</f>
+        <v>767</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>383.851</v>
       </c>
       <c r="B49">
         <v>38.909999999999997</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <f>336+221</f>
+        <v>557</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Final plots and data for the gamma ray lab
</commit_message>
<xml_diff>
--- a/gamma/data-table-shiedling.xlsx
+++ b/gamma/data-table-shiedling.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Pb" sheetId="1" r:id="rId1"/>
     <sheet name="Al" sheetId="6" r:id="rId2"/>
     <sheet name="energy-v-murho" sheetId="5" r:id="rId3"/>
     <sheet name="Error analysis" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Thickness (mm)</t>
   </si>
@@ -57,6 +58,15 @@
   </si>
   <si>
     <t>Al Data</t>
+  </si>
+  <si>
+    <t>Istope: Pb, Z: 82</t>
+  </si>
+  <si>
+    <t>g/mol</t>
+  </si>
+  <si>
+    <t>Istope: Al, Z: 13</t>
   </si>
 </sst>
 </file>
@@ -1293,8 +1303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:C25"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1905,7 +1915,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1930,11 +1940,11 @@
         <v>276.39699999999999</v>
       </c>
       <c r="B2">
-        <v>0.40810000000000002</v>
+        <v>0.40289999999999998</v>
       </c>
       <c r="C2">
         <f>(0.068)*B2</f>
-        <v>2.7750800000000003E-2</v>
+        <v>2.73972E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1942,11 +1952,11 @@
         <v>302.851</v>
       </c>
       <c r="B3">
-        <v>0.34210000000000002</v>
+        <v>0.33779999999999999</v>
       </c>
       <c r="C3">
-        <f>B3*(0.033)</f>
-        <v>1.12893E-2</v>
+        <f>B3*(0.032)</f>
+        <v>1.0809599999999999E-2</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -1957,11 +1967,11 @@
         <v>356.005</v>
       </c>
       <c r="B4">
-        <v>0.25090000000000001</v>
+        <v>0.2492</v>
       </c>
       <c r="C4">
-        <f>B4*(0.017)</f>
-        <v>4.2653000000000005E-3</v>
+        <f>B4*(0.018)</f>
+        <v>4.4856000000000002E-3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1969,11 +1979,11 @@
         <v>383.851</v>
       </c>
       <c r="B5">
-        <v>0.2041</v>
+        <v>0.20319999999999999</v>
       </c>
       <c r="C5">
         <f>B5*(0.043)</f>
-        <v>8.776299999999999E-3</v>
+        <v>8.7375999999999981E-3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1981,11 +1991,11 @@
         <v>661.7</v>
       </c>
       <c r="B6">
-        <v>9.7199999999999995E-2</v>
+        <v>9.8199999999999996E-2</v>
       </c>
       <c r="C6">
-        <f>B6*(0.0108)</f>
-        <v>1.0497600000000001E-3</v>
+        <f>B6*(0.0109)</f>
+        <v>1.0703799999999999E-3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1993,11 +2003,11 @@
         <v>1173.2</v>
       </c>
       <c r="B7">
-        <v>6.9400000000000003E-2</v>
+        <v>7.0400000000000004E-2</v>
       </c>
       <c r="C7">
-        <f>B7*(0.063)</f>
-        <v>4.3722000000000006E-3</v>
+        <f>B7*(0.054)</f>
+        <v>3.8016E-3</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2005,22 +2015,36 @@
         <v>1332.5</v>
       </c>
       <c r="B8">
-        <v>5.11E-2</v>
+        <v>5.0700000000000002E-2</v>
       </c>
       <c r="C8">
-        <f>B8*(0.04)</f>
-        <v>2.0439999999999998E-3</v>
+        <f>B8*(0.044)</f>
+        <v>2.2307999999999998E-3</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>80.998000000000005</v>
       </c>
+      <c r="B12">
+        <v>0.22259999999999999</v>
+      </c>
+      <c r="C12">
+        <f>0.252*B12</f>
+        <v>5.6095199999999998E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>276.39699999999999</v>
       </c>
+      <c r="B13">
+        <v>9.5200000000000007E-2</v>
+      </c>
+      <c r="C13">
+        <f>0.1073*B13</f>
+        <v>1.0214960000000002E-2</v>
+      </c>
       <c r="E13" t="s">
         <v>9</v>
       </c>
@@ -2029,27 +2053,48 @@
       <c r="A14">
         <v>302.851</v>
       </c>
+      <c r="B14">
+        <v>0.1547</v>
+      </c>
+      <c r="C14">
+        <f>0.1115*B14</f>
+        <v>1.7249050000000002E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>356.005</v>
       </c>
+      <c r="B15">
+        <v>0.14349999999999999</v>
+      </c>
+      <c r="C15">
+        <f>0.1091*B15</f>
+        <v>1.5655849999999999E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>383.851</v>
       </c>
+      <c r="B16">
+        <v>9.6299999999999997E-2</v>
+      </c>
+      <c r="C16">
+        <f>0.1091*B16</f>
+        <v>1.0506329999999999E-2</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>661.7</v>
       </c>
       <c r="B17">
-        <v>5.45E-2</v>
+        <v>7.5700000000000003E-2</v>
       </c>
       <c r="C17">
         <f>B17*0.0844</f>
-        <v>4.5998000000000002E-3</v>
+        <v>6.3890800000000001E-3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2057,11 +2102,11 @@
         <v>1173.2</v>
       </c>
       <c r="B18">
-        <v>7.6399999999999996E-2</v>
+        <v>0.106</v>
       </c>
       <c r="C18">
         <f>B18*0.2617</f>
-        <v>1.9993879999999999E-2</v>
+        <v>2.77402E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2069,11 +2114,11 @@
         <v>1332.5</v>
       </c>
       <c r="B19">
-        <v>7.8899999999999998E-2</v>
+        <v>0.1105</v>
       </c>
       <c r="C19">
         <f>B19*0.2155</f>
-        <v>1.7002949999999999E-2</v>
+        <v>2.3812750000000001E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2195,4 +2240,49 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>207.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>26.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>